<commit_message>
fixing root directory to open excel file
</commit_message>
<xml_diff>
--- a/static/calc/Piql_order_form.xlsx
+++ b/static/calc/Piql_order_form.xlsx
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="G4" s="59" t="n">
-        <v>44080.87444465241</v>
+        <v>44084.78196113411</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
@@ -876,7 +876,7 @@
       </c>
       <c r="G7" s="23" t="inlineStr">
         <is>
-          <t>Trujillo AS</t>
+          <t>Los marineros</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       <c r="E10" s="42" t="n"/>
       <c r="F10" s="45" t="inlineStr">
         <is>
-          <t>El texto</t>
+          <t>test</t>
         </is>
       </c>
       <c r="H10" s="28" t="n"/>
@@ -1014,9 +1014,15 @@
       <c r="C18" s="25" t="n"/>
       <c r="D18" s="25" t="n"/>
       <c r="E18" s="34" t="n"/>
-      <c r="F18" s="2" t="n"/>
-      <c r="G18" s="9" t="n"/>
-      <c r="H18" s="10" t="n"/>
+      <c r="F18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="9" t="n">
+        <v>1500</v>
+      </c>
+      <c r="H18" s="10" t="n">
+        <v>1500</v>
+      </c>
     </row>
     <row r="19" ht="17.25" customHeight="1">
       <c r="A19" s="36" t="inlineStr">
@@ -1028,9 +1034,15 @@
       <c r="C19" s="25" t="n"/>
       <c r="D19" s="25" t="n"/>
       <c r="E19" s="34" t="n"/>
-      <c r="F19" s="14" t="n"/>
-      <c r="G19" s="9" t="n"/>
-      <c r="H19" s="10" t="n"/>
+      <c r="F19" s="14" t="n">
+        <v>450</v>
+      </c>
+      <c r="G19" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="H19" s="10" t="n">
+        <v>6750</v>
+      </c>
       <c r="I19" s="16" t="n"/>
     </row>
     <row r="20" ht="17.25" customHeight="1">
@@ -1048,17 +1060,17 @@
       </c>
       <c r="E20" s="8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F20" s="15" t="n">
-        <v>89000</v>
+        <v>780000</v>
       </c>
       <c r="G20" s="11" t="n">
-        <v>0.03</v>
+        <v>0.016</v>
       </c>
       <c r="H20" s="10" t="n">
-        <v>720</v>
+        <v>12480</v>
       </c>
       <c r="I20" s="16" t="n"/>
     </row>
@@ -1072,15 +1084,9 @@
       <c r="C21" s="25" t="n"/>
       <c r="D21" s="25" t="n"/>
       <c r="E21" s="34" t="n"/>
-      <c r="F21" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9" t="n">
-        <v>8880</v>
-      </c>
-      <c r="H21" s="10" t="n">
-        <v>8880</v>
-      </c>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="9" t="n"/>
+      <c r="H21" s="10" t="n"/>
       <c r="I21" s="16" t="n"/>
     </row>
     <row r="22" ht="17.25" customHeight="1">
@@ -1096,20 +1102,10 @@
           <t>Payment:</t>
         </is>
       </c>
-      <c r="E22" s="4" t="inlineStr">
-        <is>
-          <t>yearly</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="n">
-        <v>6000</v>
-      </c>
-      <c r="G22" s="11" t="n">
-        <v>0.576</v>
-      </c>
-      <c r="H22" s="10" t="n">
-        <v>2880</v>
-      </c>
+      <c r="E22" s="4" t="n"/>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="11" t="n"/>
+      <c r="H22" s="10" t="n"/>
       <c r="I22" s="16" t="n"/>
     </row>
     <row r="23" ht="17.25" customHeight="1">
@@ -1220,15 +1216,9 @@
       <c r="C29" s="25" t="n"/>
       <c r="D29" s="25" t="n"/>
       <c r="E29" s="34" t="n"/>
-      <c r="F29" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9" t="n">
-        <v>79900</v>
-      </c>
-      <c r="H29" s="10" t="n">
-        <v>79900</v>
-      </c>
+      <c r="F29" s="2" t="n"/>
+      <c r="G29" s="9" t="n"/>
+      <c r="H29" s="10" t="n"/>
       <c r="I29" s="16" t="n"/>
     </row>
     <row r="30" ht="17.25" customHeight="1">
@@ -1241,15 +1231,9 @@
       <c r="C30" s="25" t="n"/>
       <c r="D30" s="25" t="n"/>
       <c r="E30" s="34" t="n"/>
-      <c r="F30" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="9" t="n">
-        <v>3000</v>
-      </c>
-      <c r="H30" s="10" t="n">
-        <v>3000</v>
-      </c>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="9" t="n"/>
+      <c r="H30" s="10" t="n"/>
       <c r="I30" s="16" t="n"/>
     </row>
     <row r="31">
@@ -1265,20 +1249,10 @@
           <t>Type:</t>
         </is>
       </c>
-      <c r="E31" s="6" t="inlineStr">
-        <is>
-          <t>gold</t>
-        </is>
-      </c>
-      <c r="F31" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G31" s="9" t="n">
-        <v>2500</v>
-      </c>
-      <c r="H31" s="10" t="n">
-        <v>2500</v>
-      </c>
+      <c r="E31" s="6" t="n"/>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="9" t="n"/>
+      <c r="H31" s="10" t="n"/>
       <c r="I31" s="16" t="n"/>
     </row>
     <row r="32">
@@ -1295,14 +1269,14 @@
         </is>
       </c>
       <c r="E32" s="6" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
         <v>30</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="I32" s="16" t="n"/>
     </row>
@@ -1314,7 +1288,7 @@
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>97880</v>
+        <v>13980</v>
       </c>
     </row>
     <row r="34">
@@ -1328,7 +1302,7 @@
       <c r="F34" s="41" t="n"/>
       <c r="G34" s="42" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>14260</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">

</xml_diff>

<commit_message>
changed the path to open excel order form
</commit_message>
<xml_diff>
--- a/static/calc/Piql_order_form.xlsx
+++ b/static/calc/Piql_order_form.xlsx
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="G4" s="59" t="n">
-        <v>44084.78196113411</v>
+        <v>44084.83020343081</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
@@ -876,7 +876,7 @@
       </c>
       <c r="G7" s="23" t="inlineStr">
         <is>
-          <t>Los marineros</t>
+          <t>Nueva propuesta</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       <c r="E10" s="42" t="n"/>
       <c r="F10" s="45" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>vamos</t>
         </is>
       </c>
       <c r="H10" s="28" t="n"/>
@@ -1035,13 +1035,13 @@
       <c r="D19" s="25" t="n"/>
       <c r="E19" s="34" t="n"/>
       <c r="F19" s="14" t="n">
-        <v>450</v>
+        <v>240</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>15</v>
       </c>
       <c r="H19" s="10" t="n">
-        <v>6750</v>
+        <v>3600</v>
       </c>
       <c r="I19" s="16" t="n"/>
     </row>
@@ -1058,20 +1058,10 @@
           <t>Pages/frame:</t>
         </is>
       </c>
-      <c r="E20" s="8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F20" s="15" t="n">
-        <v>780000</v>
-      </c>
-      <c r="G20" s="11" t="n">
-        <v>0.016</v>
-      </c>
-      <c r="H20" s="10" t="n">
-        <v>12480</v>
-      </c>
+      <c r="E20" s="8" t="n"/>
+      <c r="F20" s="15" t="n"/>
+      <c r="G20" s="11" t="n"/>
+      <c r="H20" s="10" t="n"/>
       <c r="I20" s="16" t="n"/>
     </row>
     <row r="21" ht="17.25" customHeight="1">
@@ -1133,9 +1123,15 @@
       <c r="C24" s="25" t="n"/>
       <c r="D24" s="25" t="n"/>
       <c r="E24" s="34" t="n"/>
-      <c r="F24" s="2" t="n"/>
-      <c r="G24" s="9" t="n"/>
-      <c r="H24" s="10" t="n"/>
+      <c r="F24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9" t="n">
+        <v>200</v>
+      </c>
+      <c r="H24" s="10" t="n">
+        <v>200</v>
+      </c>
       <c r="I24" s="16" t="n"/>
     </row>
     <row r="25" ht="16.5" customHeight="1">
@@ -1151,10 +1147,20 @@
           <t>Entity:</t>
         </is>
       </c>
-      <c r="E25" s="4" t="n"/>
-      <c r="F25" s="2" t="n"/>
-      <c r="G25" s="9" t="n"/>
-      <c r="H25" s="10" t="n"/>
+      <c r="E25" s="4" t="inlineStr">
+        <is>
+          <t>public</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9" t="n">
+        <v>500</v>
+      </c>
+      <c r="H25" s="10" t="n">
+        <v>500</v>
+      </c>
       <c r="I25" s="16" t="n"/>
     </row>
     <row r="26" ht="16.5" customHeight="1">
@@ -1167,9 +1173,15 @@
       <c r="C26" s="25" t="n"/>
       <c r="D26" s="25" t="n"/>
       <c r="E26" s="34" t="n"/>
-      <c r="F26" s="2" t="n"/>
-      <c r="G26" s="9" t="n"/>
-      <c r="H26" s="10" t="n"/>
+      <c r="F26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="H26" s="10" t="n">
+        <v>300</v>
+      </c>
       <c r="I26" s="16" t="n"/>
     </row>
     <row r="27" ht="17.5" customHeight="1">
@@ -1185,10 +1197,20 @@
           <t>Period (years):</t>
         </is>
       </c>
-      <c r="E27" s="4" t="n"/>
-      <c r="F27" s="2" t="n"/>
-      <c r="G27" s="9" t="n"/>
-      <c r="H27" s="10" t="n"/>
+      <c r="E27" s="4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="H27" s="10" t="n">
+        <v>600</v>
+      </c>
       <c r="I27" s="16" t="n"/>
     </row>
     <row r="28">
@@ -1201,9 +1223,15 @@
       <c r="C28" s="25" t="n"/>
       <c r="D28" s="25" t="n"/>
       <c r="E28" s="34" t="n"/>
-      <c r="F28" s="2" t="n"/>
-      <c r="G28" s="9" t="n"/>
-      <c r="H28" s="10" t="n"/>
+      <c r="F28" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="9" t="n">
+        <v>900</v>
+      </c>
+      <c r="H28" s="10" t="n">
+        <v>900</v>
+      </c>
       <c r="I28" s="16" t="n"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
@@ -1216,9 +1244,15 @@
       <c r="C29" s="25" t="n"/>
       <c r="D29" s="25" t="n"/>
       <c r="E29" s="34" t="n"/>
-      <c r="F29" s="2" t="n"/>
-      <c r="G29" s="9" t="n"/>
-      <c r="H29" s="10" t="n"/>
+      <c r="F29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9" t="n">
+        <v>79900</v>
+      </c>
+      <c r="H29" s="10" t="n">
+        <v>79900</v>
+      </c>
       <c r="I29" s="16" t="n"/>
     </row>
     <row r="30" ht="17.25" customHeight="1">
@@ -1231,9 +1265,15 @@
       <c r="C30" s="25" t="n"/>
       <c r="D30" s="25" t="n"/>
       <c r="E30" s="34" t="n"/>
-      <c r="F30" s="2" t="n"/>
-      <c r="G30" s="9" t="n"/>
-      <c r="H30" s="10" t="n"/>
+      <c r="F30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="9" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H30" s="10" t="n">
+        <v>3000</v>
+      </c>
       <c r="I30" s="16" t="n"/>
     </row>
     <row r="31">
@@ -1249,10 +1289,20 @@
           <t>Type:</t>
         </is>
       </c>
-      <c r="E31" s="6" t="n"/>
-      <c r="F31" s="2" t="n"/>
-      <c r="G31" s="9" t="n"/>
-      <c r="H31" s="10" t="n"/>
+      <c r="E31" s="6" t="inlineStr">
+        <is>
+          <t>gold</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="9" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H31" s="10" t="n">
+        <v>2500</v>
+      </c>
       <c r="I31" s="16" t="n"/>
     </row>
     <row r="32">
@@ -1269,14 +1319,14 @@
         </is>
       </c>
       <c r="E32" s="6" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>300</v>
+        <v>40</v>
       </c>
       <c r="I32" s="16" t="n"/>
     </row>
@@ -1288,7 +1338,7 @@
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>13980</v>
+        <v>93000</v>
       </c>
     </row>
     <row r="34">
@@ -1302,7 +1352,7 @@
       <c r="F34" s="41" t="n"/>
       <c r="G34" s="42" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="35">

</xml_diff>